<commit_message>
Refatoração Projeto 2 - Manipulação arquivos Excel
</commit_message>
<xml_diff>
--- a/Projeto 2 - Manipulação de arquivos Excel/saída/Análise de Bollinger.xlsx
+++ b/Projeto 2 - Manipulação de arquivos Excel/saída/Análise de Bollinger.xlsx
@@ -4,11 +4,12 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Dados" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Gráfico" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Dados" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Gráfico" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -658,6 +659,24 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:D1825"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -29877,13 +29896,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T36"/>
+  <dimension ref="A1:T35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -29903,11 +29922,10 @@
     <row r="33"/>
     <row r="34"/>
     <row r="35"/>
-    <row r="36"/>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="I32:L36"/>
     <mergeCell ref="A1:T2"/>
+    <mergeCell ref="I32:L35"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>

</xml_diff>